<commit_message>
[fix]: corregir el endpoint de cargar el stock del productos en megabahia
</commit_message>
<xml_diff>
--- a/appVittoria/archivo_convertido.xlsx
+++ b/appVittoria/archivo_convertido.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:AE4"/>
+  <dimension ref="A1:AE2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -593,48 +593,48 @@
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
-          <t>000000600453</t>
+          <t>HOAC01191</t>
         </is>
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t>COLADOR 12 EN 1</t>
+          <t>ESPUMA DE PUERTA DOBLE</t>
         </is>
       </c>
       <c r="C2" t="inlineStr">
         <is>
-          <t>11</t>
+          <t>86</t>
         </is>
       </c>
       <c r="D2" t="inlineStr">
         <is>
-          <t>12</t>
+          <t>86</t>
         </is>
       </c>
       <c r="E2" t="inlineStr"/>
       <c r="F2" t="inlineStr">
         <is>
-          <t>7.197500000000001</t>
+          <t>5.95</t>
         </is>
       </c>
       <c r="G2" t="inlineStr">
         <is>
-          <t>4.445178571429</t>
+          <t>5.75</t>
         </is>
       </c>
       <c r="H2" t="inlineStr">
         <is>
-          <t>3.552410714286</t>
+          <t>5.5</t>
         </is>
       </c>
       <c r="I2" t="inlineStr">
         <is>
-          <t>3.347053571429</t>
+          <t>4.95</t>
         </is>
       </c>
       <c r="J2" t="inlineStr">
         <is>
-          <t>3.2030357142860004</t>
+          <t>4.75</t>
         </is>
       </c>
       <c r="K2" t="inlineStr">
@@ -645,7 +645,7 @@
       <c r="L2" t="inlineStr"/>
       <c r="M2" t="inlineStr">
         <is>
-          <t>COCINA</t>
+          <t>ACCESORIOS PARA EL HOGAR</t>
         </is>
       </c>
       <c r="N2" t="inlineStr">
@@ -697,7 +697,7 @@
       </c>
       <c r="AC2" t="inlineStr">
         <is>
-          <t>HOCO</t>
+          <t>HOAC</t>
         </is>
       </c>
       <c r="AD2" t="inlineStr">
@@ -706,248 +706,6 @@
         </is>
       </c>
       <c r="AE2" t="inlineStr">
-        <is>
-          <t>HOGAR</t>
-        </is>
-      </c>
-    </row>
-    <row r="3">
-      <c r="A3" t="inlineStr">
-        <is>
-          <t>009283044565</t>
-        </is>
-      </c>
-      <c r="B3" t="inlineStr">
-        <is>
-          <t>VENDAS DE BOX</t>
-        </is>
-      </c>
-      <c r="C3" t="inlineStr">
-        <is>
-          <t>207</t>
-        </is>
-      </c>
-      <c r="D3" t="inlineStr">
-        <is>
-          <t>207</t>
-        </is>
-      </c>
-      <c r="E3" t="inlineStr"/>
-      <c r="F3" t="inlineStr">
-        <is>
-          <t>5</t>
-        </is>
-      </c>
-      <c r="G3" t="inlineStr">
-        <is>
-          <t>3.9</t>
-        </is>
-      </c>
-      <c r="H3" t="inlineStr">
-        <is>
-          <t>3.75</t>
-        </is>
-      </c>
-      <c r="I3" t="inlineStr">
-        <is>
-          <t>3.25</t>
-        </is>
-      </c>
-      <c r="J3" t="inlineStr">
-        <is>
-          <t>2.95</t>
-        </is>
-      </c>
-      <c r="K3" t="inlineStr">
-        <is>
-          <t>0</t>
-        </is>
-      </c>
-      <c r="L3" t="inlineStr"/>
-      <c r="M3" t="inlineStr">
-        <is>
-          <t>ACCESORIOS PARA EJERCICIOS</t>
-        </is>
-      </c>
-      <c r="N3" t="inlineStr">
-        <is>
-          <t>NORMAL</t>
-        </is>
-      </c>
-      <c r="O3" t="inlineStr">
-        <is>
-          <t>1</t>
-        </is>
-      </c>
-      <c r="P3" t="inlineStr">
-        <is>
-          <t>0</t>
-        </is>
-      </c>
-      <c r="Q3" t="inlineStr">
-        <is>
-          <t>0</t>
-        </is>
-      </c>
-      <c r="R3" t="inlineStr">
-        <is>
-          <t>IVA 15%</t>
-        </is>
-      </c>
-      <c r="S3" t="inlineStr">
-        <is>
-          <t>15</t>
-        </is>
-      </c>
-      <c r="T3" t="inlineStr">
-        <is>
-          <t>NO</t>
-        </is>
-      </c>
-      <c r="U3" t="inlineStr"/>
-      <c r="V3" t="inlineStr"/>
-      <c r="W3" t="inlineStr"/>
-      <c r="X3" t="inlineStr"/>
-      <c r="Y3" t="inlineStr"/>
-      <c r="Z3" t="inlineStr"/>
-      <c r="AA3" t="inlineStr"/>
-      <c r="AB3" t="inlineStr">
-        <is>
-          <t>NO</t>
-        </is>
-      </c>
-      <c r="AC3" t="inlineStr">
-        <is>
-          <t>DEEJ</t>
-        </is>
-      </c>
-      <c r="AD3" t="inlineStr">
-        <is>
-          <t>DE</t>
-        </is>
-      </c>
-      <c r="AE3" t="inlineStr">
-        <is>
-          <t>DEPORTES</t>
-        </is>
-      </c>
-    </row>
-    <row r="4">
-      <c r="A4" t="inlineStr">
-        <is>
-          <t>17874117802</t>
-        </is>
-      </c>
-      <c r="B4" t="inlineStr">
-        <is>
-          <t>DISPENSADOR DE JUGO X3</t>
-        </is>
-      </c>
-      <c r="C4" t="inlineStr">
-        <is>
-          <t>6</t>
-        </is>
-      </c>
-      <c r="D4" t="inlineStr">
-        <is>
-          <t>6</t>
-        </is>
-      </c>
-      <c r="E4" t="inlineStr"/>
-      <c r="F4" t="inlineStr">
-        <is>
-          <t>34.25276785714001</t>
-        </is>
-      </c>
-      <c r="G4" t="inlineStr">
-        <is>
-          <t>31.15160714286</t>
-        </is>
-      </c>
-      <c r="H4" t="inlineStr">
-        <is>
-          <t>27.40410714286</t>
-        </is>
-      </c>
-      <c r="I4" t="inlineStr">
-        <is>
-          <t>24.895552321430003</t>
-        </is>
-      </c>
-      <c r="J4" t="inlineStr">
-        <is>
-          <t>23.803571741069998</t>
-        </is>
-      </c>
-      <c r="K4" t="inlineStr">
-        <is>
-          <t>0</t>
-        </is>
-      </c>
-      <c r="L4" t="inlineStr"/>
-      <c r="M4" t="inlineStr">
-        <is>
-          <t>ACCESORIOS PARA EL HOGAR</t>
-        </is>
-      </c>
-      <c r="N4" t="inlineStr">
-        <is>
-          <t>NORMAL</t>
-        </is>
-      </c>
-      <c r="O4" t="inlineStr">
-        <is>
-          <t>1</t>
-        </is>
-      </c>
-      <c r="P4" t="inlineStr">
-        <is>
-          <t>0</t>
-        </is>
-      </c>
-      <c r="Q4" t="inlineStr">
-        <is>
-          <t>0</t>
-        </is>
-      </c>
-      <c r="R4" t="inlineStr">
-        <is>
-          <t>IVA 15%</t>
-        </is>
-      </c>
-      <c r="S4" t="inlineStr">
-        <is>
-          <t>15</t>
-        </is>
-      </c>
-      <c r="T4" t="inlineStr">
-        <is>
-          <t>NO</t>
-        </is>
-      </c>
-      <c r="U4" t="inlineStr"/>
-      <c r="V4" t="inlineStr"/>
-      <c r="W4" t="inlineStr"/>
-      <c r="X4" t="inlineStr"/>
-      <c r="Y4" t="inlineStr"/>
-      <c r="Z4" t="inlineStr"/>
-      <c r="AA4" t="inlineStr"/>
-      <c r="AB4" t="inlineStr">
-        <is>
-          <t>NO</t>
-        </is>
-      </c>
-      <c r="AC4" t="inlineStr">
-        <is>
-          <t>HOAC</t>
-        </is>
-      </c>
-      <c r="AD4" t="inlineStr">
-        <is>
-          <t>HO</t>
-        </is>
-      </c>
-      <c r="AE4" t="inlineStr">
         <is>
           <t>HOGAR</t>
         </is>

</xml_diff>

<commit_message>
feat: filtrar gmb y reportes de gd
</commit_message>
<xml_diff>
--- a/appVittoria/archivo_convertido.xlsx
+++ b/appVittoria/archivo_convertido.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:AE2"/>
+  <dimension ref="A1:AE4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -593,48 +593,48 @@
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
-          <t>HOAC01191</t>
+          <t>000000600453</t>
         </is>
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t>ESPUMA DE PUERTA DOBLE</t>
+          <t>COLADOR 12 EN 1</t>
         </is>
       </c>
       <c r="C2" t="inlineStr">
         <is>
-          <t>86</t>
+          <t>11</t>
         </is>
       </c>
       <c r="D2" t="inlineStr">
         <is>
-          <t>86</t>
+          <t>12</t>
         </is>
       </c>
       <c r="E2" t="inlineStr"/>
       <c r="F2" t="inlineStr">
         <is>
-          <t>5.95</t>
+          <t>7.197500000000001</t>
         </is>
       </c>
       <c r="G2" t="inlineStr">
         <is>
-          <t>5.75</t>
+          <t>4.445178571429</t>
         </is>
       </c>
       <c r="H2" t="inlineStr">
         <is>
-          <t>5.5</t>
+          <t>3.552410714286</t>
         </is>
       </c>
       <c r="I2" t="inlineStr">
         <is>
-          <t>4.95</t>
+          <t>3.347053571429</t>
         </is>
       </c>
       <c r="J2" t="inlineStr">
         <is>
-          <t>4.75</t>
+          <t>3.2030357142860004</t>
         </is>
       </c>
       <c r="K2" t="inlineStr">
@@ -645,7 +645,7 @@
       <c r="L2" t="inlineStr"/>
       <c r="M2" t="inlineStr">
         <is>
-          <t>ACCESORIOS PARA EL HOGAR</t>
+          <t>COCINA</t>
         </is>
       </c>
       <c r="N2" t="inlineStr">
@@ -697,15 +697,257 @@
       </c>
       <c r="AC2" t="inlineStr">
         <is>
+          <t>HOCO</t>
+        </is>
+      </c>
+      <c r="AD2" t="inlineStr">
+        <is>
+          <t>HO</t>
+        </is>
+      </c>
+      <c r="AE2" t="inlineStr">
+        <is>
+          <t>HOGAR</t>
+        </is>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" t="inlineStr">
+        <is>
+          <t>009283044565</t>
+        </is>
+      </c>
+      <c r="B3" t="inlineStr">
+        <is>
+          <t>VENDAS DE BOX</t>
+        </is>
+      </c>
+      <c r="C3" t="inlineStr">
+        <is>
+          <t>207</t>
+        </is>
+      </c>
+      <c r="D3" t="inlineStr">
+        <is>
+          <t>207</t>
+        </is>
+      </c>
+      <c r="E3" t="inlineStr"/>
+      <c r="F3" t="inlineStr">
+        <is>
+          <t>5</t>
+        </is>
+      </c>
+      <c r="G3" t="inlineStr">
+        <is>
+          <t>3.9</t>
+        </is>
+      </c>
+      <c r="H3" t="inlineStr">
+        <is>
+          <t>3.75</t>
+        </is>
+      </c>
+      <c r="I3" t="inlineStr">
+        <is>
+          <t>3.25</t>
+        </is>
+      </c>
+      <c r="J3" t="inlineStr">
+        <is>
+          <t>2.95</t>
+        </is>
+      </c>
+      <c r="K3" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="L3" t="inlineStr"/>
+      <c r="M3" t="inlineStr">
+        <is>
+          <t>ACCESORIOS PARA EJERCICIOS</t>
+        </is>
+      </c>
+      <c r="N3" t="inlineStr">
+        <is>
+          <t>NORMAL</t>
+        </is>
+      </c>
+      <c r="O3" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
+      <c r="P3" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="Q3" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="R3" t="inlineStr">
+        <is>
+          <t>IVA 15%</t>
+        </is>
+      </c>
+      <c r="S3" t="inlineStr">
+        <is>
+          <t>15</t>
+        </is>
+      </c>
+      <c r="T3" t="inlineStr">
+        <is>
+          <t>NO</t>
+        </is>
+      </c>
+      <c r="U3" t="inlineStr"/>
+      <c r="V3" t="inlineStr"/>
+      <c r="W3" t="inlineStr"/>
+      <c r="X3" t="inlineStr"/>
+      <c r="Y3" t="inlineStr"/>
+      <c r="Z3" t="inlineStr"/>
+      <c r="AA3" t="inlineStr"/>
+      <c r="AB3" t="inlineStr">
+        <is>
+          <t>NO</t>
+        </is>
+      </c>
+      <c r="AC3" t="inlineStr">
+        <is>
+          <t>DEEJ</t>
+        </is>
+      </c>
+      <c r="AD3" t="inlineStr">
+        <is>
+          <t>DE</t>
+        </is>
+      </c>
+      <c r="AE3" t="inlineStr">
+        <is>
+          <t>DEPORTES</t>
+        </is>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" t="inlineStr">
+        <is>
+          <t>17874117802</t>
+        </is>
+      </c>
+      <c r="B4" t="inlineStr">
+        <is>
+          <t>DISPENSADOR DE JUGO X3</t>
+        </is>
+      </c>
+      <c r="C4" t="inlineStr">
+        <is>
+          <t>6</t>
+        </is>
+      </c>
+      <c r="D4" t="inlineStr">
+        <is>
+          <t>6</t>
+        </is>
+      </c>
+      <c r="E4" t="inlineStr"/>
+      <c r="F4" t="inlineStr">
+        <is>
+          <t>34.25276785714001</t>
+        </is>
+      </c>
+      <c r="G4" t="inlineStr">
+        <is>
+          <t>31.15160714286</t>
+        </is>
+      </c>
+      <c r="H4" t="inlineStr">
+        <is>
+          <t>27.40410714286</t>
+        </is>
+      </c>
+      <c r="I4" t="inlineStr">
+        <is>
+          <t>24.895552321430003</t>
+        </is>
+      </c>
+      <c r="J4" t="inlineStr">
+        <is>
+          <t>23.803571741069998</t>
+        </is>
+      </c>
+      <c r="K4" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="L4" t="inlineStr"/>
+      <c r="M4" t="inlineStr">
+        <is>
+          <t>ACCESORIOS PARA EL HOGAR</t>
+        </is>
+      </c>
+      <c r="N4" t="inlineStr">
+        <is>
+          <t>NORMAL</t>
+        </is>
+      </c>
+      <c r="O4" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
+      <c r="P4" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="Q4" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="R4" t="inlineStr">
+        <is>
+          <t>IVA 15%</t>
+        </is>
+      </c>
+      <c r="S4" t="inlineStr">
+        <is>
+          <t>15</t>
+        </is>
+      </c>
+      <c r="T4" t="inlineStr">
+        <is>
+          <t>NO</t>
+        </is>
+      </c>
+      <c r="U4" t="inlineStr"/>
+      <c r="V4" t="inlineStr"/>
+      <c r="W4" t="inlineStr"/>
+      <c r="X4" t="inlineStr"/>
+      <c r="Y4" t="inlineStr"/>
+      <c r="Z4" t="inlineStr"/>
+      <c r="AA4" t="inlineStr"/>
+      <c r="AB4" t="inlineStr">
+        <is>
+          <t>NO</t>
+        </is>
+      </c>
+      <c r="AC4" t="inlineStr">
+        <is>
           <t>HOAC</t>
         </is>
       </c>
-      <c r="AD2" t="inlineStr">
+      <c r="AD4" t="inlineStr">
         <is>
           <t>HO</t>
         </is>
       </c>
-      <c r="AE2" t="inlineStr">
+      <c r="AE4" t="inlineStr">
         <is>
           <t>HOGAR</t>
         </is>

</xml_diff>

<commit_message>
feat: email a realizar pedido
</commit_message>
<xml_diff>
--- a/appVittoria/archivo_convertido.xlsx
+++ b/appVittoria/archivo_convertido.xlsx
@@ -1,13 +1,13 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <workbookPr/>
   <workbookProtection/>
   <bookViews>
     <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" tabRatio="600" firstSheet="0" activeTab="0" autoFilterDateGrouping="1"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" state="visible" r:id="rId1"/>
+    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Sheet1" sheetId="1" state="visible" r:id="rId1"/>
   </sheets>
   <definedNames/>
   <calcPr calcId="124519" fullCalcOnLoad="1"/>
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:AE4"/>
+  <dimension ref="A1:AE3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -593,96 +593,56 @@
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
-          <t>000000600453</t>
+          <t>MB001002</t>
         </is>
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t>COLADOR 12 EN 1</t>
-        </is>
-      </c>
-      <c r="C2" t="inlineStr">
-        <is>
-          <t>11</t>
-        </is>
-      </c>
+          <t>Peluche saco para dormir infan</t>
+        </is>
+      </c>
+      <c r="C2" t="inlineStr"/>
       <c r="D2" t="inlineStr">
         <is>
-          <t>12</t>
+          <t>50</t>
         </is>
       </c>
       <c r="E2" t="inlineStr"/>
       <c r="F2" t="inlineStr">
         <is>
-          <t>7.197500000000001</t>
+          <t>20</t>
         </is>
       </c>
       <c r="G2" t="inlineStr">
         <is>
-          <t>4.445178571429</t>
+          <t>19</t>
         </is>
       </c>
       <c r="H2" t="inlineStr">
         <is>
-          <t>3.552410714286</t>
+          <t>18</t>
         </is>
       </c>
       <c r="I2" t="inlineStr">
         <is>
-          <t>3.347053571429</t>
+          <t>17</t>
         </is>
       </c>
       <c r="J2" t="inlineStr">
         <is>
-          <t>3.2030357142860004</t>
-        </is>
-      </c>
-      <c r="K2" t="inlineStr">
-        <is>
-          <t>0</t>
-        </is>
-      </c>
+          <t>16</t>
+        </is>
+      </c>
+      <c r="K2" t="inlineStr"/>
       <c r="L2" t="inlineStr"/>
-      <c r="M2" t="inlineStr">
-        <is>
-          <t>COCINA</t>
-        </is>
-      </c>
-      <c r="N2" t="inlineStr">
-        <is>
-          <t>NORMAL</t>
-        </is>
-      </c>
-      <c r="O2" t="inlineStr">
-        <is>
-          <t>1</t>
-        </is>
-      </c>
-      <c r="P2" t="inlineStr">
-        <is>
-          <t>0</t>
-        </is>
-      </c>
-      <c r="Q2" t="inlineStr">
-        <is>
-          <t>0</t>
-        </is>
-      </c>
-      <c r="R2" t="inlineStr">
-        <is>
-          <t>IVA 15%</t>
-        </is>
-      </c>
-      <c r="S2" t="inlineStr">
-        <is>
-          <t>15</t>
-        </is>
-      </c>
-      <c r="T2" t="inlineStr">
-        <is>
-          <t>NO</t>
-        </is>
-      </c>
+      <c r="M2" t="inlineStr"/>
+      <c r="N2" t="inlineStr"/>
+      <c r="O2" t="inlineStr"/>
+      <c r="P2" t="inlineStr"/>
+      <c r="Q2" t="inlineStr"/>
+      <c r="R2" t="inlineStr"/>
+      <c r="S2" t="inlineStr"/>
+      <c r="T2" t="inlineStr"/>
       <c r="U2" t="inlineStr"/>
       <c r="V2" t="inlineStr"/>
       <c r="W2" t="inlineStr"/>
@@ -690,120 +650,64 @@
       <c r="Y2" t="inlineStr"/>
       <c r="Z2" t="inlineStr"/>
       <c r="AA2" t="inlineStr"/>
-      <c r="AB2" t="inlineStr">
-        <is>
-          <t>NO</t>
-        </is>
-      </c>
-      <c r="AC2" t="inlineStr">
-        <is>
-          <t>HOCO</t>
-        </is>
-      </c>
-      <c r="AD2" t="inlineStr">
-        <is>
-          <t>HO</t>
-        </is>
-      </c>
-      <c r="AE2" t="inlineStr">
-        <is>
-          <t>HOGAR</t>
-        </is>
-      </c>
+      <c r="AB2" t="inlineStr"/>
+      <c r="AC2" t="inlineStr"/>
+      <c r="AD2" t="inlineStr"/>
+      <c r="AE2" t="inlineStr"/>
     </row>
     <row r="3">
       <c r="A3" t="inlineStr">
         <is>
-          <t>009283044565</t>
+          <t>LapHP</t>
         </is>
       </c>
       <c r="B3" t="inlineStr">
         <is>
-          <t>VENDAS DE BOX</t>
-        </is>
-      </c>
-      <c r="C3" t="inlineStr">
-        <is>
-          <t>207</t>
-        </is>
-      </c>
+          <t>Laptop HP</t>
+        </is>
+      </c>
+      <c r="C3" t="inlineStr"/>
       <c r="D3" t="inlineStr">
         <is>
-          <t>207</t>
+          <t>75</t>
         </is>
       </c>
       <c r="E3" t="inlineStr"/>
       <c r="F3" t="inlineStr">
         <is>
-          <t>5</t>
+          <t>1000</t>
         </is>
       </c>
       <c r="G3" t="inlineStr">
         <is>
-          <t>3.9</t>
+          <t>1250.3</t>
         </is>
       </c>
       <c r="H3" t="inlineStr">
         <is>
-          <t>3.75</t>
+          <t>1180.99</t>
         </is>
       </c>
       <c r="I3" t="inlineStr">
         <is>
-          <t>3.25</t>
+          <t>0</t>
         </is>
       </c>
       <c r="J3" t="inlineStr">
         <is>
-          <t>2.95</t>
-        </is>
-      </c>
-      <c r="K3" t="inlineStr">
-        <is>
           <t>0</t>
         </is>
       </c>
+      <c r="K3" t="inlineStr"/>
       <c r="L3" t="inlineStr"/>
-      <c r="M3" t="inlineStr">
-        <is>
-          <t>ACCESORIOS PARA EJERCICIOS</t>
-        </is>
-      </c>
-      <c r="N3" t="inlineStr">
-        <is>
-          <t>NORMAL</t>
-        </is>
-      </c>
-      <c r="O3" t="inlineStr">
-        <is>
-          <t>1</t>
-        </is>
-      </c>
-      <c r="P3" t="inlineStr">
-        <is>
-          <t>0</t>
-        </is>
-      </c>
-      <c r="Q3" t="inlineStr">
-        <is>
-          <t>0</t>
-        </is>
-      </c>
-      <c r="R3" t="inlineStr">
-        <is>
-          <t>IVA 15%</t>
-        </is>
-      </c>
-      <c r="S3" t="inlineStr">
-        <is>
-          <t>15</t>
-        </is>
-      </c>
-      <c r="T3" t="inlineStr">
-        <is>
-          <t>NO</t>
-        </is>
-      </c>
+      <c r="M3" t="inlineStr"/>
+      <c r="N3" t="inlineStr"/>
+      <c r="O3" t="inlineStr"/>
+      <c r="P3" t="inlineStr"/>
+      <c r="Q3" t="inlineStr"/>
+      <c r="R3" t="inlineStr"/>
+      <c r="S3" t="inlineStr"/>
+      <c r="T3" t="inlineStr"/>
       <c r="U3" t="inlineStr"/>
       <c r="V3" t="inlineStr"/>
       <c r="W3" t="inlineStr"/>
@@ -811,147 +715,10 @@
       <c r="Y3" t="inlineStr"/>
       <c r="Z3" t="inlineStr"/>
       <c r="AA3" t="inlineStr"/>
-      <c r="AB3" t="inlineStr">
-        <is>
-          <t>NO</t>
-        </is>
-      </c>
-      <c r="AC3" t="inlineStr">
-        <is>
-          <t>DEEJ</t>
-        </is>
-      </c>
-      <c r="AD3" t="inlineStr">
-        <is>
-          <t>DE</t>
-        </is>
-      </c>
-      <c r="AE3" t="inlineStr">
-        <is>
-          <t>DEPORTES</t>
-        </is>
-      </c>
-    </row>
-    <row r="4">
-      <c r="A4" t="inlineStr">
-        <is>
-          <t>17874117802</t>
-        </is>
-      </c>
-      <c r="B4" t="inlineStr">
-        <is>
-          <t>DISPENSADOR DE JUGO X3</t>
-        </is>
-      </c>
-      <c r="C4" t="inlineStr">
-        <is>
-          <t>6</t>
-        </is>
-      </c>
-      <c r="D4" t="inlineStr">
-        <is>
-          <t>6</t>
-        </is>
-      </c>
-      <c r="E4" t="inlineStr"/>
-      <c r="F4" t="inlineStr">
-        <is>
-          <t>34.25276785714001</t>
-        </is>
-      </c>
-      <c r="G4" t="inlineStr">
-        <is>
-          <t>31.15160714286</t>
-        </is>
-      </c>
-      <c r="H4" t="inlineStr">
-        <is>
-          <t>27.40410714286</t>
-        </is>
-      </c>
-      <c r="I4" t="inlineStr">
-        <is>
-          <t>24.895552321430003</t>
-        </is>
-      </c>
-      <c r="J4" t="inlineStr">
-        <is>
-          <t>23.803571741069998</t>
-        </is>
-      </c>
-      <c r="K4" t="inlineStr">
-        <is>
-          <t>0</t>
-        </is>
-      </c>
-      <c r="L4" t="inlineStr"/>
-      <c r="M4" t="inlineStr">
-        <is>
-          <t>ACCESORIOS PARA EL HOGAR</t>
-        </is>
-      </c>
-      <c r="N4" t="inlineStr">
-        <is>
-          <t>NORMAL</t>
-        </is>
-      </c>
-      <c r="O4" t="inlineStr">
-        <is>
-          <t>1</t>
-        </is>
-      </c>
-      <c r="P4" t="inlineStr">
-        <is>
-          <t>0</t>
-        </is>
-      </c>
-      <c r="Q4" t="inlineStr">
-        <is>
-          <t>0</t>
-        </is>
-      </c>
-      <c r="R4" t="inlineStr">
-        <is>
-          <t>IVA 15%</t>
-        </is>
-      </c>
-      <c r="S4" t="inlineStr">
-        <is>
-          <t>15</t>
-        </is>
-      </c>
-      <c r="T4" t="inlineStr">
-        <is>
-          <t>NO</t>
-        </is>
-      </c>
-      <c r="U4" t="inlineStr"/>
-      <c r="V4" t="inlineStr"/>
-      <c r="W4" t="inlineStr"/>
-      <c r="X4" t="inlineStr"/>
-      <c r="Y4" t="inlineStr"/>
-      <c r="Z4" t="inlineStr"/>
-      <c r="AA4" t="inlineStr"/>
-      <c r="AB4" t="inlineStr">
-        <is>
-          <t>NO</t>
-        </is>
-      </c>
-      <c r="AC4" t="inlineStr">
-        <is>
-          <t>HOAC</t>
-        </is>
-      </c>
-      <c r="AD4" t="inlineStr">
-        <is>
-          <t>HO</t>
-        </is>
-      </c>
-      <c r="AE4" t="inlineStr">
-        <is>
-          <t>HOGAR</t>
-        </is>
-      </c>
+      <c r="AB3" t="inlineStr"/>
+      <c r="AC3" t="inlineStr"/>
+      <c r="AD3" t="inlineStr"/>
+      <c r="AE3" t="inlineStr"/>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>

</xml_diff>